<commit_message>
flask version on web app
</commit_message>
<xml_diff>
--- a/test_requests.xlsx
+++ b/test_requests.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,11 @@
           <t>Notes</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Request ID</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -486,25 +491,96 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
+      <c r="D2" t="n">
+        <v>12</v>
+      </c>
+      <c r="E2" t="n">
+        <v>20</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2024-02-20</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>example</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Transmittance</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Tool B</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nopthing</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Transmittance</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Tool A</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
         <is>
           <t>20</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2024-02-20</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>example</t>
-        </is>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testing out git and where it commits
</commit_message>
<xml_diff>
--- a/test_requests.xlsx
+++ b/test_requests.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,6 +474,91 @@
           <t>Request ID</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Measurement Tool (Images)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Voltage (Images)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Expected Value (Images)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Polarisers (Images)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Cell Orientation</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Polariser Number</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>State of Cell</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Measurement Tool (Test B)</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Voltage (Test B)</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Expected Value (Test B)</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Test B Field 1</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Test B Field 2</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Measurement Tool (Test C)</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Voltage (Test C)</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Expected Value (Test C)</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Test C Field 1</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Test C Field 2</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -508,6 +593,23 @@
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -542,6 +644,23 @@
       <c r="H3" t="n">
         <v>2</v>
       </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -559,15 +678,11 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+      <c r="D4" t="n">
+        <v>20</v>
+      </c>
+      <c r="E4" t="n">
+        <v>30</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -581,6 +696,132 @@
       </c>
       <c r="H4" t="n">
         <v>3</v>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Transmittance</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-01-29</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>42421</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>4</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Tool A</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Tool A</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>Tool A</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
configured test instances instead of the previous version
</commit_message>
<xml_diff>
--- a/test_requests.xlsx
+++ b/test_requests.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:AB6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -557,6 +557,21 @@
       <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Test C Field 2</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Instance ID</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Voltage</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Tool</t>
         </is>
       </c>
     </row>
@@ -610,6 +625,9 @@
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
       <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -661,6 +679,9 @@
       <c r="W3" t="inlineStr"/>
       <c r="X3" t="inlineStr"/>
       <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -714,6 +735,9 @@
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr"/>
       <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -743,84 +767,129 @@
           <t>Tool A</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="J5" t="n">
+        <v>2</v>
+      </c>
+      <c r="K5" t="n">
+        <v>12</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
+      <c r="M5" t="n">
+        <v>45</v>
+      </c>
+      <c r="N5" t="n">
+        <v>2</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Tool A</t>
+        </is>
+      </c>
+      <c r="Q5" t="n">
+        <v>3</v>
+      </c>
+      <c r="R5" t="n">
+        <v>4</v>
+      </c>
+      <c r="S5" t="n">
+        <v>5</v>
+      </c>
+      <c r="T5" t="n">
+        <v>6</v>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>Tool A</t>
+        </is>
+      </c>
+      <c r="V5" t="n">
+        <v>5</v>
+      </c>
+      <c r="W5" t="n">
+        <v>5</v>
+      </c>
+      <c r="X5" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>7</v>
+      </c>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr"/>
+      <c r="AB5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Images</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>1a8db2d3-13dc-445d-a5c8-984531af9298</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
         <is>
           <t>45</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>ON</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>Tool A</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>Tool A</t>
-        </is>
-      </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="X5" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>7</t>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>OFF</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>5b6c39e6-031d-43a7-960d-c49668764a6c</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>CS-160S</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
made the UI more centered and added more sections and fields to the test instances
</commit_message>
<xml_diff>
--- a/test_requests.xlsx
+++ b/test_requests.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB6"/>
+  <dimension ref="A1:AN7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -572,6 +572,66 @@
       <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Tool</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Polarisers Type</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Polarisers Lamination</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Number of Polarisers</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Orientation of Pol1</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Orientation of Cell Alignment Axis</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Orientation of Pol2</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>Voltage Range</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Voltage Single Point</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Voltage Sweep</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>Tool Setup</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>Tool Angle of Incidence</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>Sample Number</t>
         </is>
       </c>
     </row>
@@ -628,6 +688,18 @@
       <c r="Z2" t="inlineStr"/>
       <c r="AA2" t="inlineStr"/>
       <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="inlineStr"/>
+      <c r="AJ2" t="inlineStr"/>
+      <c r="AK2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="inlineStr"/>
+      <c r="AN2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -682,6 +754,18 @@
       <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="inlineStr"/>
       <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="inlineStr"/>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="inlineStr"/>
+      <c r="AK3" t="inlineStr"/>
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="inlineStr"/>
+      <c r="AN3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -738,6 +822,18 @@
       <c r="Z4" t="inlineStr"/>
       <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="inlineStr"/>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr"/>
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="inlineStr"/>
+      <c r="AK4" t="inlineStr"/>
+      <c r="AL4" t="inlineStr"/>
+      <c r="AM4" t="inlineStr"/>
+      <c r="AN4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -826,6 +922,18 @@
       <c r="Z5" t="inlineStr"/>
       <c r="AA5" t="inlineStr"/>
       <c r="AB5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="inlineStr"/>
+      <c r="AE5" t="inlineStr"/>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="inlineStr"/>
+      <c r="AH5" t="inlineStr"/>
+      <c r="AI5" t="inlineStr"/>
+      <c r="AJ5" t="inlineStr"/>
+      <c r="AK5" t="inlineStr"/>
+      <c r="AL5" t="inlineStr"/>
+      <c r="AM5" t="inlineStr"/>
+      <c r="AN5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -852,15 +960,11 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="M6" t="n">
+        <v>45</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -882,14 +986,126 @@
           <t>5b6c39e6-031d-43a7-960d-c49668764a6c</t>
         </is>
       </c>
-      <c r="AA6" t="inlineStr">
+      <c r="AA6" t="n">
+        <v>50</v>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>CS-160S</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="inlineStr"/>
+      <c r="AE6" t="inlineStr"/>
+      <c r="AF6" t="inlineStr"/>
+      <c r="AG6" t="inlineStr"/>
+      <c r="AH6" t="inlineStr"/>
+      <c r="AI6" t="inlineStr"/>
+      <c r="AJ6" t="inlineStr"/>
+      <c r="AK6" t="inlineStr"/>
+      <c r="AL6" t="inlineStr"/>
+      <c r="AM6" t="inlineStr"/>
+      <c r="AN6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Images</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>31cdb862-d715-45fd-b3d5-d163917dec02</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
+      <c r="X7" t="inlineStr"/>
+      <c r="Y7" t="inlineStr"/>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>f4d2fe47-fdc7-4bdd-b2d8-9b526637c3ac</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr"/>
+      <c r="AB7" t="inlineStr"/>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>loose</t>
+        </is>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="AH7" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="AI7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AJ7" t="inlineStr">
         <is>
           <t>50</t>
         </is>
       </c>
-      <c r="AB6" t="inlineStr">
-        <is>
-          <t>CS-160S</t>
+      <c r="AK7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AL7" t="inlineStr">
+        <is>
+          <t>Nikon camera</t>
+        </is>
+      </c>
+      <c r="AM7" t="inlineStr">
+        <is>
+          <t>on axis</t>
+        </is>
+      </c>
+      <c r="AN7" t="inlineStr">
+        <is>
+          <t>4</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added some dropdown options instead of just typing in the values
</commit_message>
<xml_diff>
--- a/test_requests.xlsx
+++ b/test_requests.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -756,10 +756,8 @@
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="O5" t="n">
+        <v>6</v>
       </c>
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
@@ -784,6 +782,178 @@
         </is>
       </c>
       <c r="V5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>d65f8b92-b7a5-4a0c-a564-28db06bff5b3</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Transmission</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>f457e8d4-a2c6-419b-893a-f1757920464e</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>exampe</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>R534</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>Moonfish</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>2025-02-14</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>UV-VIS</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>d65f8b92-b7a5-4a0c-a564-28db06bff5b3</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Transmission</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>fd9685e2-9f0f-4202-96dc-60b55ac4646f</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>exampe</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>R534</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>Moonfish</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>2025-02-14</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>UV-VIS</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>d65f8b92-b7a5-4a0c-a564-28db06bff5b3</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Custom or New</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>427b4aad-8d57-4242-86e0-f109805e423b</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>exampe</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>R534</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>Moonfish</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>2025-02-14</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>